<commit_message>
MENT-69: Add health facility from Ile and Alto Molocue
</commit_message>
<xml_diff>
--- a/mentoring-core/add-health-facilities_20171129.xlsx
+++ b/mentoring-core/add-health-facilities_20171129.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="2000" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>Solicitador</t>
   </si>
@@ -129,6 +129,21 @@
   </si>
   <si>
     <t>Health_Facility</t>
+  </si>
+  <si>
+    <t>CS Welele</t>
+  </si>
+  <si>
+    <t>Alto Molocué</t>
+  </si>
+  <si>
+    <t>CS Mucuaba</t>
+  </si>
+  <si>
+    <t>CS Curruane</t>
+  </si>
+  <si>
+    <t>Timoteo Salua</t>
   </si>
 </sst>
 </file>
@@ -466,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F20"/>
+  <dimension ref="B3:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -786,6 +801,57 @@
         <v>43066</v>
       </c>
     </row>
+    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="3">
+        <v>43145</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="3">
+        <v>43145</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="3">
+        <v>43145</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>